<commit_message>
Added celing and floor for predictions, and ability to run for all centers in the nba
</commit_message>
<xml_diff>
--- a/TeamStats/CenterVsLeague.xlsx
+++ b/TeamStats/CenterVsLeague.xlsx
@@ -503,37 +503,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.223876324076725</v>
+        <v>1.041842594156392</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9152375148718841</v>
+        <v>0.8668508590562275</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9639872662156785</v>
+        <v>1.059969488327278</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8450610727562401</v>
+        <v>0.8345514565355882</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9410709410709411</v>
+        <v>0.9965167348175072</v>
       </c>
       <c r="G2" t="n">
-        <v>1.075237611550461</v>
+        <v>1.151663952159856</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9524946287896873</v>
+        <v>1.099290487583533</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7450610543035839</v>
+        <v>0.8175637659414855</v>
       </c>
       <c r="J2" t="n">
-        <v>1.281618887015177</v>
+        <v>1.323461803693204</v>
       </c>
       <c r="K2" t="n">
-        <v>37.74107142857143</v>
+        <v>41.92258064516129</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9771384711888834</v>
+        <v>0.9929916605574656</v>
       </c>
     </row>
     <row r="3">
@@ -543,37 +543,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9715983691520974</v>
+        <v>0.9395525940028558</v>
       </c>
       <c r="C3" t="n">
-        <v>1.067333487430569</v>
+        <v>1.059244959521477</v>
       </c>
       <c r="D3" t="n">
-        <v>1.186245317452694</v>
+        <v>1.172540589466538</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9437892577874633</v>
+        <v>1.006814101517872</v>
       </c>
       <c r="F3" t="n">
-        <v>1.061249337111406</v>
+        <v>1.082390809503486</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8118947128771825</v>
+        <v>0.8283037610467903</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9446744758439591</v>
+        <v>0.953782550569635</v>
       </c>
       <c r="I3" t="n">
-        <v>1.120030672641442</v>
+        <v>1.097681025369979</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8617782171308949</v>
+        <v>0.7992334269056358</v>
       </c>
       <c r="K3" t="n">
-        <v>38.47413793103448</v>
+        <v>42.26136363636363</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9961179928183159</v>
+        <v>1.001016182899018</v>
       </c>
     </row>
     <row r="4">
@@ -583,37 +583,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.721442885771543</v>
+        <v>0.7599322451493687</v>
       </c>
       <c r="C4" t="n">
-        <v>1.045433001557316</v>
+        <v>1.062051649928264</v>
       </c>
       <c r="D4" t="n">
-        <v>1.095636025998143</v>
+        <v>1.138054101541052</v>
       </c>
       <c r="E4" t="n">
-        <v>1.047087980173482</v>
+        <v>1.052772204034217</v>
       </c>
       <c r="F4" t="n">
-        <v>1.024054357387691</v>
+        <v>1.090306545153273</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9751142712036566</v>
+        <v>0.9844186355778181</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8402960133683457</v>
+        <v>0.9651722581615766</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9265693768820941</v>
+        <v>0.9563953488372093</v>
       </c>
       <c r="J4" t="n">
-        <v>1.034288926363125</v>
+        <v>1.13773229006567</v>
       </c>
       <c r="K4" t="n">
-        <v>38.44210526315789</v>
+        <v>43.84705882352941</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9952886482625771</v>
+        <v>1.038575466531131</v>
       </c>
     </row>
     <row r="5">
@@ -623,37 +623,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.015364061456246</v>
+        <v>1.060008054772453</v>
       </c>
       <c r="C5" t="n">
-        <v>1.050849752860722</v>
+        <v>1.012020594266765</v>
       </c>
       <c r="D5" t="n">
-        <v>1.151346332404828</v>
+        <v>1.047269158967977</v>
       </c>
       <c r="E5" t="n">
-        <v>1.022304832713755</v>
+        <v>0.9995856925838973</v>
       </c>
       <c r="F5" t="n">
-        <v>1.162374495707829</v>
+        <v>1.13534769872798</v>
       </c>
       <c r="G5" t="n">
-        <v>1.164719823937701</v>
+        <v>1.239638281838734</v>
       </c>
       <c r="H5" t="n">
-        <v>1.069467653377894</v>
+        <v>1.035608892386386</v>
       </c>
       <c r="I5" t="n">
-        <v>1.047023395876766</v>
+        <v>1.05448717948718</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9668353007307475</v>
+        <v>1.021925817650283</v>
       </c>
       <c r="K5" t="n">
-        <v>41.66315789473685</v>
+        <v>44.63589743589743</v>
       </c>
       <c r="L5" t="n">
-        <v>1.078683589765411</v>
+        <v>1.057260150335241</v>
       </c>
     </row>
     <row r="6">
@@ -663,37 +663,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8063185193917246</v>
+        <v>0.7535994764397906</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9383725052076487</v>
+        <v>0.9252930610701455</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8717024414222514</v>
+        <v>0.8615691765193942</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8378890589693127</v>
+        <v>0.8958408138839018</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9112856171679701</v>
+        <v>0.9081681446704921</v>
       </c>
       <c r="G6" t="n">
-        <v>1.059560441749071</v>
+        <v>1.156995729716152</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9035803387958191</v>
+        <v>0.7888427109974424</v>
       </c>
       <c r="I6" t="n">
-        <v>1.056289089645587</v>
+        <v>1.089228036175711</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8544125913434513</v>
+        <v>0.7814726840855106</v>
       </c>
       <c r="K6" t="n">
-        <v>34.82156862745098</v>
+        <v>37.41666666666666</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9015508316297465</v>
+        <v>0.8862631401520572</v>
       </c>
     </row>
     <row r="7">
@@ -703,37 +703,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.316531367820387</v>
+        <v>1.550261780104712</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9053319424217698</v>
+        <v>0.8837492909812819</v>
       </c>
       <c r="D7" t="n">
-        <v>0.849188738334671</v>
+        <v>0.8598630989421281</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9397643500724593</v>
+        <v>0.8404308797127469</v>
       </c>
       <c r="F7" t="n">
-        <v>1.012784741598301</v>
+        <v>1.136384976525822</v>
       </c>
       <c r="G7" t="n">
-        <v>1.046732833495451</v>
+        <v>1.083798040693293</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9286630440499937</v>
+        <v>0.9195652173913043</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9309666552808565</v>
+        <v>0.9563953488372093</v>
       </c>
       <c r="J7" t="n">
-        <v>1.107840054877526</v>
+        <v>1.038242280285036</v>
       </c>
       <c r="K7" t="n">
-        <v>37.44576271186441</v>
+        <v>41.86857142857142</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9694927553400907</v>
+        <v>0.9917123809701491</v>
       </c>
     </row>
     <row r="8">
@@ -743,37 +743,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5943594506085341</v>
+        <v>0.6178579558388345</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9714481057059199</v>
+        <v>0.8945288416483761</v>
       </c>
       <c r="D8" t="n">
-        <v>1.1187354213375</v>
+        <v>1.028097183517762</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8269108713391966</v>
+        <v>0.8474748263211302</v>
       </c>
       <c r="F8" t="n">
-        <v>1.099813782740612</v>
+        <v>1.141661563584405</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9225928724498011</v>
+        <v>0.6144294092591985</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9027126795498082</v>
+        <v>0.8917352385188481</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7857760301022051</v>
+        <v>0.8108569261880688</v>
       </c>
       <c r="J8" t="n">
-        <v>0.7502159338625426</v>
+        <v>0.968346586801611</v>
       </c>
       <c r="K8" t="n">
-        <v>36.86341463414634</v>
+        <v>38.57826086956521</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9544154221107422</v>
+        <v>0.9137770321567777</v>
       </c>
     </row>
     <row r="9">
@@ -783,37 +783,37 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7615230460921844</v>
+        <v>0.8839211904105815</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8900822669104204</v>
+        <v>0.9465735737528734</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9261838440111421</v>
+        <v>0.969770412340746</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9215264869888476</v>
+        <v>0.9606066332797883</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9185321685321686</v>
+        <v>0.9111790626801746</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8443372270187912</v>
+        <v>0.822075913219371</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8561112437335879</v>
+        <v>0.8552715708709113</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9655142460041696</v>
+        <v>0.9941477968176256</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9812394603709949</v>
+        <v>1.048818602325291</v>
       </c>
       <c r="K9" t="n">
-        <v>34.0453125</v>
+        <v>38.47105263157895</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8814531052823638</v>
+        <v>0.9112376635247633</v>
       </c>
     </row>
     <row r="10">
@@ -823,37 +823,37 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3888628320470728</v>
+        <v>0.3478151429722111</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9722492339474719</v>
+        <v>0.9474235350582486</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9008475078527827</v>
+        <v>1.00396103585276</v>
       </c>
       <c r="E10" t="n">
-        <v>1.209760341691055</v>
+        <v>1.117718547161994</v>
       </c>
       <c r="F10" t="n">
-        <v>1.080074271563633</v>
+        <v>1.064388467557482</v>
       </c>
       <c r="G10" t="n">
-        <v>1.149735798493673</v>
+        <v>1.115674453654861</v>
       </c>
       <c r="H10" t="n">
-        <v>0.895557259895471</v>
+        <v>0.946611253196931</v>
       </c>
       <c r="I10" t="n">
-        <v>1.000103499770822</v>
+        <v>1.085140876565295</v>
       </c>
       <c r="J10" t="n">
-        <v>1.00893401743748</v>
+        <v>0.7664443632377124</v>
       </c>
       <c r="K10" t="n">
-        <v>38.03404255319149</v>
+        <v>40.01538461538461</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9847236654077475</v>
+        <v>0.947817205085695</v>
       </c>
     </row>
     <row r="11">
@@ -863,37 +863,37 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.311511912714318</v>
+        <v>1.384162303664922</v>
       </c>
       <c r="C11" t="n">
-        <v>1.097794930823572</v>
+        <v>1.11468377765173</v>
       </c>
       <c r="D11" t="n">
-        <v>1.234911792014856</v>
+        <v>1.217408214063472</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9319496076001652</v>
+        <v>0.8606822262118491</v>
       </c>
       <c r="F11" t="n">
-        <v>1.002821002821003</v>
+        <v>1.00674882629108</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8577394052254388</v>
+        <v>0.8500376789751318</v>
       </c>
       <c r="H11" t="n">
-        <v>1.108723906527678</v>
+        <v>1.036764705882353</v>
       </c>
       <c r="I11" t="n">
-        <v>1.232337271253185</v>
+        <v>1.178415697674419</v>
       </c>
       <c r="J11" t="n">
-        <v>1.49522203485104</v>
+        <v>1.590855106888361</v>
       </c>
       <c r="K11" t="n">
-        <v>41.25555555555556</v>
+        <v>45.37142857142857</v>
       </c>
       <c r="L11" t="n">
-        <v>1.068130526180176</v>
+        <v>1.074682176184385</v>
       </c>
     </row>
     <row r="12">
@@ -903,37 +903,37 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8884435537742151</v>
+        <v>0.7382198952879581</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9091114270882705</v>
+        <v>0.8997447532614862</v>
       </c>
       <c r="D12" t="n">
-        <v>1.18590735582379</v>
+        <v>1.257622899813317</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9123296158612144</v>
+        <v>1.046319569120287</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9067653512097956</v>
+        <v>0.9623109024517476</v>
       </c>
       <c r="G12" t="n">
-        <v>1.522487444275154</v>
+        <v>1.558402411454408</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9373756664279462</v>
+        <v>0.7212276214833759</v>
       </c>
       <c r="I12" t="n">
-        <v>1.11497181684812</v>
+        <v>1.001937984496124</v>
       </c>
       <c r="J12" t="n">
-        <v>1.103616263818625</v>
+        <v>1.283847980997625</v>
       </c>
       <c r="K12" t="n">
-        <v>38.11944444444444</v>
+        <v>42.08571428571428</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9869347704531747</v>
+        <v>0.9968556961710316</v>
       </c>
     </row>
     <row r="13">
@@ -943,37 +943,37 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9372591336519193</v>
+        <v>0.8477994109947644</v>
       </c>
       <c r="C13" t="n">
-        <v>1.015328364505695</v>
+        <v>0.9840958238797505</v>
       </c>
       <c r="D13" t="n">
-        <v>1.173844725376759</v>
+        <v>1.12281230553827</v>
       </c>
       <c r="E13" t="n">
-        <v>1.14097798112668</v>
+        <v>1.129645421903052</v>
       </c>
       <c r="F13" t="n">
-        <v>1.005481005481005</v>
+        <v>1.009621967918623</v>
       </c>
       <c r="G13" t="n">
-        <v>1.247021135289292</v>
+        <v>1.255133760361718</v>
       </c>
       <c r="H13" t="n">
-        <v>0.976917567989423</v>
+        <v>0.8775875159846547</v>
       </c>
       <c r="I13" t="n">
-        <v>1.005505960335703</v>
+        <v>0.9265079941860466</v>
       </c>
       <c r="J13" t="n">
-        <v>1.035153716435335</v>
+        <v>1.135577494061758</v>
       </c>
       <c r="K13" t="n">
-        <v>40.33076923076923</v>
+        <v>43.128125</v>
       </c>
       <c r="L13" t="n">
-        <v>1.044187265923552</v>
+        <v>1.021546569925268</v>
       </c>
     </row>
     <row r="14">
@@ -983,37 +983,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.110554442217769</v>
+        <v>1.02459830294277</v>
       </c>
       <c r="C14" t="n">
-        <v>1.138533414584603</v>
+        <v>1.192075615623839</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9629371711544413</v>
+        <v>1.027176362036779</v>
       </c>
       <c r="E14" t="n">
-        <v>1.103624535315985</v>
+        <v>1.112078251717947</v>
       </c>
       <c r="F14" t="n">
-        <v>1.002821002821003</v>
+        <v>1.065242026873887</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9006263754867108</v>
+        <v>0.8976691006418418</v>
       </c>
       <c r="H14" t="n">
-        <v>0.8920187793427231</v>
+        <v>0.8269247729076638</v>
       </c>
       <c r="I14" t="n">
-        <v>1.111304146397962</v>
+        <v>0.9399057738572575</v>
       </c>
       <c r="J14" t="n">
-        <v>1.041315345699831</v>
+        <v>1.091367024326316</v>
       </c>
       <c r="K14" t="n">
-        <v>39.6375</v>
+        <v>44.83448275862069</v>
       </c>
       <c r="L14" t="n">
-        <v>1.026238118995961</v>
+        <v>1.061963905837375</v>
       </c>
     </row>
     <row r="15">
@@ -1023,37 +1023,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.309819639278557</v>
+        <v>1.324181937172775</v>
       </c>
       <c r="C15" t="n">
-        <v>1.09607962624416</v>
+        <v>1.049702212138401</v>
       </c>
       <c r="D15" t="n">
-        <v>1.065552460538533</v>
+        <v>1.005732731798382</v>
       </c>
       <c r="E15" t="n">
-        <v>1.144237918215613</v>
+        <v>1.107495511669659</v>
       </c>
       <c r="F15" t="n">
-        <v>1.12039312039312</v>
+        <v>1.100528169014085</v>
       </c>
       <c r="G15" t="n">
-        <v>1.034433722701879</v>
+        <v>1.041296156744536</v>
       </c>
       <c r="H15" t="n">
-        <v>1.400620673191693</v>
+        <v>1.388363171355499</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9612230715774844</v>
+        <v>0.9205305232558141</v>
       </c>
       <c r="J15" t="n">
-        <v>1.23035413153457</v>
+        <v>1.230819477434679</v>
       </c>
       <c r="K15" t="n">
-        <v>44.278</v>
+        <v>47.38500000000001</v>
       </c>
       <c r="L15" t="n">
-        <v>1.14638338525142</v>
+        <v>1.122376273392568</v>
       </c>
     </row>
     <row r="16">
@@ -1063,37 +1063,37 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8915391759128012</v>
+        <v>0.8612565445026178</v>
       </c>
       <c r="C16" t="n">
-        <v>1.031692949470628</v>
+        <v>1.021191781685259</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9121996512444234</v>
+        <v>0.8416649381179562</v>
       </c>
       <c r="E16" t="n">
-        <v>1.059479553903346</v>
+        <v>1.089447436664672</v>
       </c>
       <c r="F16" t="n">
-        <v>1.025593220715172</v>
+        <v>1.00113023821944</v>
       </c>
       <c r="G16" t="n">
-        <v>1.073220280196707</v>
+        <v>1.046805660219375</v>
       </c>
       <c r="H16" t="n">
-        <v>1.035464544189486</v>
+        <v>1.156969309462915</v>
       </c>
       <c r="I16" t="n">
-        <v>1.056289089645587</v>
+        <v>1.062661498708011</v>
       </c>
       <c r="J16" t="n">
-        <v>1.000287911816724</v>
+        <v>0.9985484296648192</v>
       </c>
       <c r="K16" t="n">
-        <v>38.99756097560976</v>
+        <v>42.4111111111111</v>
       </c>
       <c r="L16" t="n">
-        <v>1.009669722385117</v>
+        <v>1.004563149505687</v>
       </c>
     </row>
     <row r="17">
@@ -1103,37 +1103,37 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.085170340681363</v>
+        <v>1.148342059336824</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8452163315051796</v>
+        <v>0.8760477721056281</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7188950789229341</v>
+        <v>0.6767441056488972</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8299256505576209</v>
+        <v>0.7678635547576301</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9544089544089545</v>
+        <v>0.9367718657624761</v>
       </c>
       <c r="G17" t="n">
-        <v>0.8298628745556119</v>
+        <v>0.8815205559742108</v>
       </c>
       <c r="H17" t="n">
-        <v>0.8345667223681069</v>
+        <v>0.8239023870417732</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9440583738707437</v>
+        <v>0.9563953488372093</v>
       </c>
       <c r="J17" t="n">
-        <v>0.8650927487352446</v>
+        <v>0.8031802586434416</v>
       </c>
       <c r="K17" t="n">
-        <v>33.1375</v>
+        <v>36.25</v>
       </c>
       <c r="L17" t="n">
-        <v>0.8579493073031517</v>
+        <v>0.8586291001473161</v>
       </c>
     </row>
     <row r="18">
@@ -1143,37 +1143,37 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.655484882809096</v>
+        <v>1.500253335585205</v>
       </c>
       <c r="C18" t="n">
-        <v>1.167898683199533</v>
+        <v>1.200949627650815</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7363449194622744</v>
+        <v>0.7627817813196298</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9366413447551317</v>
+        <v>0.9946024208026872</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9742548872983655</v>
+        <v>0.988212428694028</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8726566122728376</v>
+        <v>0.9597199601332134</v>
       </c>
       <c r="H18" t="n">
-        <v>1.072788981493975</v>
+        <v>1.109469103209306</v>
       </c>
       <c r="I18" t="n">
-        <v>0.8955494455690848</v>
+        <v>0.9101181545386348</v>
       </c>
       <c r="J18" t="n">
-        <v>0.9751448053376347</v>
+        <v>0.7940770822159221</v>
       </c>
       <c r="K18" t="n">
-        <v>40.52608695652174</v>
+        <v>44.98387096774194</v>
       </c>
       <c r="L18" t="n">
-        <v>1.049244156380388</v>
+        <v>1.065502362763455</v>
       </c>
     </row>
     <row r="19">
@@ -1183,37 +1183,37 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.431663326653307</v>
+        <v>1.93782722513089</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9849278894982734</v>
+        <v>1.054700794100964</v>
       </c>
       <c r="D19" t="n">
-        <v>0.973816155988858</v>
+        <v>0.9980553827006845</v>
       </c>
       <c r="E19" t="n">
-        <v>1.10185873605948</v>
+        <v>1.025224416517056</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9793065793065793</v>
+        <v>0.9699726134585289</v>
       </c>
       <c r="G19" t="n">
-        <v>1.034433722701879</v>
+        <v>0.9562923888470234</v>
       </c>
       <c r="H19" t="n">
-        <v>1.386106469324421</v>
+        <v>1.487531969309463</v>
       </c>
       <c r="I19" t="n">
-        <v>1.172480889506602</v>
+        <v>1.332122093023256</v>
       </c>
       <c r="J19" t="n">
-        <v>1.127824620573356</v>
+        <v>1.255938242280285</v>
       </c>
       <c r="K19" t="n">
-        <v>40.75</v>
+        <v>46.69285714285714</v>
       </c>
       <c r="L19" t="n">
-        <v>1.055041396381846</v>
+        <v>1.105981956189755</v>
       </c>
     </row>
     <row r="20">
@@ -1223,37 +1223,37 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.523046092184369</v>
+        <v>1.578970331588133</v>
       </c>
       <c r="C20" t="n">
-        <v>1.136779125810204</v>
+        <v>1.301112371588832</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9943445598041699</v>
+        <v>1.035020396874784</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9952686718485976</v>
+        <v>1.089447436664672</v>
       </c>
       <c r="F20" t="n">
-        <v>1.034257397893761</v>
+        <v>0.9629919434301282</v>
       </c>
       <c r="G20" t="n">
-        <v>0.8070548040075719</v>
+        <v>0.8539730386000167</v>
       </c>
       <c r="H20" t="n">
-        <v>1.030838342845982</v>
+        <v>1.250461778914464</v>
       </c>
       <c r="I20" t="n">
-        <v>0.9962726640975426</v>
+        <v>0.9563953488372093</v>
       </c>
       <c r="J20" t="n">
-        <v>1.252491185037559</v>
+        <v>1.345869622591713</v>
       </c>
       <c r="K20" t="n">
-        <v>41.34318181818182</v>
+        <v>49.12962962962963</v>
       </c>
       <c r="L20" t="n">
-        <v>1.070399221504861</v>
+        <v>1.163700129088546</v>
       </c>
     </row>
     <row r="21">
@@ -1263,37 +1263,37 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.7845995020343718</v>
+        <v>0.7645848915482424</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8467367151096583</v>
+        <v>0.8397617697107204</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7591232660870544</v>
+        <v>0.8210063116721487</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8721978145769967</v>
+        <v>0.9402410874583226</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8969851394093817</v>
+        <v>0.8616141292197631</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8304476968773565</v>
+        <v>0.8652169232425448</v>
       </c>
       <c r="H21" t="n">
-        <v>0.8851465237237498</v>
+        <v>0.8757763975155279</v>
       </c>
       <c r="I21" t="n">
-        <v>0.8082211973803357</v>
+        <v>0.8002491694352161</v>
       </c>
       <c r="J21" t="n">
-        <v>0.7184833154479022</v>
+        <v>0.7176789955887343</v>
       </c>
       <c r="K21" t="n">
-        <v>32.45</v>
+        <v>35.48163265306123</v>
       </c>
       <c r="L21" t="n">
-        <v>0.8401495291433351</v>
+        <v>0.8404293052870506</v>
       </c>
     </row>
     <row r="22">
@@ -1303,37 +1303,37 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.698062792251169</v>
+        <v>0.8477994109947644</v>
       </c>
       <c r="C22" t="n">
-        <v>1.022750355474304</v>
+        <v>0.9753483054452637</v>
       </c>
       <c r="D22" t="n">
-        <v>1.132002476013618</v>
+        <v>1.055635500933416</v>
       </c>
       <c r="E22" t="n">
-        <v>1.184557001239157</v>
+        <v>1.262544883303411</v>
       </c>
       <c r="F22" t="n">
-        <v>1.132496132496132</v>
+        <v>1.146383509389671</v>
       </c>
       <c r="G22" t="n">
-        <v>1.174030810902319</v>
+        <v>1.185404107008289</v>
       </c>
       <c r="H22" t="n">
-        <v>0.9978515158749105</v>
+        <v>0.995913922634271</v>
       </c>
       <c r="I22" t="n">
-        <v>1.144313180449386</v>
+        <v>1.18055050872093</v>
       </c>
       <c r="J22" t="n">
-        <v>0.6408094435075885</v>
+        <v>0.7326306413301662</v>
       </c>
       <c r="K22" t="n">
-        <v>39.70416666666667</v>
+        <v>43.228125</v>
       </c>
       <c r="L22" t="n">
-        <v>1.027964158090247</v>
+        <v>1.023915201925674</v>
       </c>
     </row>
     <row r="23">
@@ -1343,37 +1343,37 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.004562316121605</v>
+        <v>0.9119186941792425</v>
       </c>
       <c r="C23" t="n">
-        <v>1.018233995012555</v>
+        <v>0.9220913549764772</v>
       </c>
       <c r="D23" t="n">
-        <v>1.02846757146526</v>
+        <v>0.9122497163146528</v>
       </c>
       <c r="E23" t="n">
-        <v>1.006881278177648</v>
+        <v>0.8859964093357271</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9152672982460216</v>
+        <v>0.9313035073184204</v>
       </c>
       <c r="G23" t="n">
-        <v>1.133311001372335</v>
+        <v>1.050046544616339</v>
       </c>
       <c r="H23" t="n">
-        <v>0.9032775811014664</v>
+        <v>0.9651722581615766</v>
       </c>
       <c r="I23" t="n">
-        <v>1.033814853695681</v>
+        <v>1.06891244870041</v>
       </c>
       <c r="J23" t="n">
-        <v>1.336155860930716</v>
+        <v>1.206685762190862</v>
       </c>
       <c r="K23" t="n">
-        <v>38.75531914893617</v>
+        <v>39.62352941176471</v>
       </c>
       <c r="L23" t="n">
-        <v>1.003397939438472</v>
+        <v>0.9385355973374964</v>
       </c>
     </row>
     <row r="24">
@@ -1383,37 +1383,37 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.184591405032287</v>
+        <v>1.325881785615872</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8119108342549334</v>
+        <v>0.7771479535480789</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6207228584201658</v>
+        <v>0.557617987095929</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9548395979622746</v>
+        <v>0.8953226873287347</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9451876118542785</v>
+        <v>0.8705316695494606</v>
       </c>
       <c r="G24" t="n">
-        <v>0.9864003160092545</v>
+        <v>0.9395153293935667</v>
       </c>
       <c r="H24" t="n">
-        <v>0.9608940523239879</v>
+        <v>0.8884860008076457</v>
       </c>
       <c r="I24" t="n">
-        <v>0.7237536354979024</v>
+        <v>0.7424648102815178</v>
       </c>
       <c r="J24" t="n">
-        <v>0.9730810068078196</v>
+        <v>0.9871233904238029</v>
       </c>
       <c r="K24" t="n">
-        <v>34.76851851851852</v>
+        <v>36.13421052631579</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9001773332001437</v>
+        <v>0.8558864736205297</v>
       </c>
     </row>
     <row r="25">
@@ -1423,37 +1423,37 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.099977733244266</v>
+        <v>1.291884816753927</v>
       </c>
       <c r="C25" t="n">
-        <v>1.020606224750039</v>
+        <v>1.051701644923426</v>
       </c>
       <c r="D25" t="n">
-        <v>1.156504694109151</v>
+        <v>1.140634723086497</v>
       </c>
       <c r="E25" t="n">
-        <v>1.092179540134931</v>
+        <v>1.093572710951526</v>
       </c>
       <c r="F25" t="n">
-        <v>1.070700329959589</v>
+        <v>1.033411580594679</v>
       </c>
       <c r="G25" t="n">
-        <v>0.8148524349641668</v>
+        <v>0.7437829691032404</v>
       </c>
       <c r="H25" t="n">
-        <v>1.263273299558809</v>
+        <v>1.397378516624041</v>
       </c>
       <c r="I25" t="n">
-        <v>1.281239543921962</v>
+        <v>1.325290697674419</v>
       </c>
       <c r="J25" t="n">
-        <v>0.9730810068078196</v>
+        <v>0.9377672209026129</v>
       </c>
       <c r="K25" t="n">
-        <v>39.9074074074074</v>
+        <v>44.35142857142857</v>
       </c>
       <c r="L25" t="n">
-        <v>1.033226180051297</v>
+        <v>1.050522129780239</v>
       </c>
     </row>
     <row r="26">
@@ -1463,37 +1463,37 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.099977733244266</v>
+        <v>0.898702481220123</v>
       </c>
       <c r="C26" t="n">
-        <v>1.209289728485341</v>
+        <v>1.326580186934326</v>
       </c>
       <c r="D26" t="n">
-        <v>1.097699370679872</v>
+        <v>1.081504829414789</v>
       </c>
       <c r="E26" t="n">
-        <v>1.059479553903346</v>
+        <v>0.9553352587620013</v>
       </c>
       <c r="F26" t="n">
-        <v>1.060454393787727</v>
+        <v>1.029733959311424</v>
       </c>
       <c r="G26" t="n">
-        <v>0.7934089498335307</v>
+        <v>0.8731365289472822</v>
       </c>
       <c r="H26" t="n">
-        <v>1.290151454868571</v>
+        <v>1.193553319248304</v>
       </c>
       <c r="I26" t="n">
-        <v>1.11497181684812</v>
+        <v>1.039560161779575</v>
       </c>
       <c r="J26" t="n">
-        <v>0.9256136406220723</v>
+        <v>1.070277806464939</v>
       </c>
       <c r="K26" t="n">
-        <v>42.21666666666667</v>
+        <v>47.1608695652174</v>
       </c>
       <c r="L26" t="n">
-        <v>1.093014256456121</v>
+        <v>1.117067448191657</v>
       </c>
     </row>
     <row r="27">
@@ -1503,37 +1503,37 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.7615230460921844</v>
+        <v>0.5872203712517848</v>
       </c>
       <c r="C27" t="n">
-        <v>1.00036563071298</v>
+        <v>1.022134275253958</v>
       </c>
       <c r="D27" t="n">
-        <v>1.086722376973073</v>
+        <v>1.200458222549075</v>
       </c>
       <c r="E27" t="n">
-        <v>0.974721189591078</v>
+        <v>0.9880202382895381</v>
       </c>
       <c r="F27" t="n">
-        <v>1.001437801437801</v>
+        <v>0.9985298999383507</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8337227018791266</v>
+        <v>0.9015551140645338</v>
       </c>
       <c r="H27" t="n">
-        <v>1.052279780377178</v>
+        <v>0.9083643338758428</v>
       </c>
       <c r="I27" t="n">
-        <v>1.045726198749131</v>
+        <v>0.970886187455955</v>
       </c>
       <c r="J27" t="n">
-        <v>0.8715008431703204</v>
+        <v>0.6749082271647593</v>
       </c>
       <c r="K27" t="n">
-        <v>37.19</v>
+        <v>40.18484848484848</v>
       </c>
       <c r="L27" t="n">
-        <v>0.9628709087470149</v>
+        <v>0.9518311805269432</v>
       </c>
     </row>
     <row r="28">
@@ -1543,37 +1543,37 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.9324771992965524</v>
+        <v>0.5684293193717278</v>
       </c>
       <c r="C28" t="n">
-        <v>1.080641885029453</v>
+        <v>1.024509359047079</v>
       </c>
       <c r="D28" t="n">
-        <v>0.9432853921512896</v>
+        <v>0.8844306160547604</v>
       </c>
       <c r="E28" t="n">
-        <v>1.073894241711554</v>
+        <v>1.091547576301616</v>
       </c>
       <c r="F28" t="n">
-        <v>1.041635327349613</v>
+        <v>0.9782472613458528</v>
       </c>
       <c r="G28" t="n">
-        <v>1.087053409479587</v>
+        <v>1.219804069329314</v>
       </c>
       <c r="H28" t="n">
-        <v>1.177427762702121</v>
+        <v>1.09806905370844</v>
       </c>
       <c r="I28" t="n">
-        <v>1.131738310334558</v>
+        <v>1.109418604651163</v>
       </c>
       <c r="J28" t="n">
-        <v>1.124685962074543</v>
+        <v>1.031543942992874</v>
       </c>
       <c r="K28" t="n">
-        <v>40.77755102040816</v>
+        <v>42.11600000000001</v>
       </c>
       <c r="L28" t="n">
-        <v>1.055754708456525</v>
+        <v>0.997573053291155</v>
       </c>
     </row>
     <row r="29">
@@ -1583,37 +1583,37 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8283233132932533</v>
+        <v>0.6799393772389087</v>
       </c>
       <c r="C29" t="n">
-        <v>0.9398063511409032</v>
+        <v>0.9060587515299878</v>
       </c>
       <c r="D29" t="n">
-        <v>1.145156298359641</v>
+        <v>1.139480234500377</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9417596034696406</v>
+        <v>1.03521685722385</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9488276154942821</v>
+        <v>0.9416646075282102</v>
       </c>
       <c r="G29" t="n">
-        <v>0.9073980023700695</v>
+        <v>0.7829294411613056</v>
       </c>
       <c r="H29" t="n">
-        <v>0.8402960133683457</v>
+        <v>0.8635751783550949</v>
       </c>
       <c r="I29" t="n">
-        <v>1.019226314570304</v>
+        <v>1.044484394124847</v>
       </c>
       <c r="J29" t="n">
-        <v>0.6520517144463182</v>
+        <v>0.6169521190148768</v>
       </c>
       <c r="K29" t="n">
-        <v>35.08070175438596</v>
+        <v>37.17894736842105</v>
       </c>
       <c r="L29" t="n">
-        <v>0.9082599402454589</v>
+        <v>0.8806324447826701</v>
       </c>
     </row>
     <row r="30">
@@ -1623,37 +1623,37 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.740941342143747</v>
+        <v>0.6459424083769634</v>
       </c>
       <c r="C30" t="n">
-        <v>1.059780072577148</v>
+        <v>1.049702212138401</v>
       </c>
       <c r="D30" t="n">
-        <v>1.296895781575447</v>
+        <v>1.429168062802164</v>
       </c>
       <c r="E30" t="n">
-        <v>1.202652466592987</v>
+        <v>1.240394973070018</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9944096430582917</v>
+        <v>0.9307210786084026</v>
       </c>
       <c r="G30" t="n">
-        <v>1.314427683142767</v>
+        <v>1.230102602747667</v>
       </c>
       <c r="H30" t="n">
-        <v>1.078758395540444</v>
+        <v>1.019427503442849</v>
       </c>
       <c r="I30" t="n">
-        <v>1.07056326653269</v>
+        <v>0.9747875670840788</v>
       </c>
       <c r="J30" t="n">
-        <v>0.9005970557403947</v>
+        <v>0.856614288324502</v>
       </c>
       <c r="K30" t="n">
-        <v>41.22702702702702</v>
+        <v>43.99230769230769</v>
       </c>
       <c r="L30" t="n">
-        <v>1.067391905847036</v>
+        <v>1.042015877717241</v>
       </c>
     </row>
     <row r="31">
@@ -1663,37 +1663,37 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.9635597726064374</v>
+        <v>0.8751477790913696</v>
       </c>
       <c r="C31" t="n">
-        <v>1.124749717071472</v>
+        <v>1.160315993632555</v>
       </c>
       <c r="D31" t="n">
-        <v>1.144903643908817</v>
+        <v>1.188750828030592</v>
       </c>
       <c r="E31" t="n">
-        <v>1.109930961232076</v>
+        <v>1.108924538136329</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8525037096465669</v>
+        <v>0.9093215205209754</v>
       </c>
       <c r="G31" t="n">
-        <v>1.228842984629098</v>
+        <v>1.271628947176508</v>
       </c>
       <c r="H31" t="n">
-        <v>0.9034351386770989</v>
+        <v>0.8957181750680637</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8083845073818269</v>
+        <v>0.8484152288072019</v>
       </c>
       <c r="J31" t="n">
-        <v>1.229307912034966</v>
+        <v>1.361274998084438</v>
       </c>
       <c r="K31" t="n">
-        <v>40.73877551020409</v>
+        <v>45.81290322580645</v>
       </c>
       <c r="L31" t="n">
-        <v>1.054750787758829</v>
+        <v>1.085139086121663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>